<commit_message>
Add showing how full shelf is, Next add the same for the other stands
</commit_message>
<xml_diff>
--- a/GuildManager2d/CSV/building.xlsx
+++ b/GuildManager2d/CSV/building.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GodotProjects\Shopper_2d\CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\MedievalStoreManager\GuildManager2d\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFF07D1-D155-4DFA-BBA4-68759F2F1E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C8DCB1-D354-4571-A85C-C740F9D4C09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="3460" windowWidth="19420" windowHeight="10560" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21150" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
   </bookViews>
   <sheets>
     <sheet name="shop_item" sheetId="1" r:id="rId1"/>
@@ -79,13 +79,13 @@
     <t>unlocked</t>
   </si>
   <si>
-    <t>res://Asset/Building/shelf.png</t>
-  </si>
-  <si>
-    <t>res://Asset/Building/stand.png</t>
-  </si>
-  <si>
-    <t>res://Asset/Building/hang.png</t>
+    <t>res://Asset/Building/Shelf/simple_shelf.png</t>
+  </si>
+  <si>
+    <t>res://Asset/Building/Hanger/simple_hanger.png</t>
+  </si>
+  <si>
+    <t>res://Asset/Building/Stand/simple_stand.png</t>
   </si>
 </sst>
 </file>
@@ -934,13 +934,13 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -1001,7 +1001,7 @@
         <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1021,7 +1021,7 @@
         <v>200</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <v>1</v>

</xml_diff>

<commit_message>
Established the license upgrades completely buildings and products are now unlocked by them, Next: Checkout minigame
</commit_message>
<xml_diff>
--- a/GuildManager2d/CSV/building.xlsx
+++ b/GuildManager2d/CSV/building.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\MedievalStoreManager\GuildManager2d\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C8DCB1-D354-4571-A85C-C740F9D4C09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5EDCBB5F-7C34-4B36-B28E-587470FDECC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21150" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
+    <workbookView xWindow="19200" yWindow="10275" windowWidth="19200" windowHeight="10875" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
   </bookViews>
   <sheets>
-    <sheet name="shop_item" sheetId="1" r:id="rId1"/>
+    <sheet name="building" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="building" localSheetId="0">shop_item!$D$5:$J$8</definedName>
+    <definedName name="building" localSheetId="0">building!$D$5:$J$8</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -49,36 +49,21 @@
     <t>name</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>stand</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
     <t>Shelf</t>
   </si>
   <si>
-    <t>shelf</t>
-  </si>
-  <si>
     <t>Stand</t>
   </si>
   <si>
     <t>Hanger</t>
   </si>
   <si>
-    <t>line</t>
-  </si>
-  <si>
     <t>sprite_path</t>
   </si>
   <si>
-    <t>unlocked</t>
-  </si>
-  <si>
     <t>res://Asset/Building/Shelf/simple_shelf.png</t>
   </si>
   <si>
@@ -86,6 +71,30 @@
   </si>
   <si>
     <t>res://Asset/Building/Stand/simple_stand.png</t>
+  </si>
+  <si>
+    <t>store_area</t>
+  </si>
+  <si>
+    <t>Beverages</t>
+  </si>
+  <si>
+    <t>Weapons</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>placeable_type</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Food,Drink,Material,Craft</t>
+  </si>
+  <si>
+    <t>Meat,Medicine</t>
   </si>
 </sst>
 </file>
@@ -569,9 +578,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -931,17 +949,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A1F4D6-F08C-4BFA-8F0D-CD932C622A30}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" customWidth="1"/>
@@ -955,16 +974,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -972,19 +991,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3">
         <v>300</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -992,19 +1011,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3">
         <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,20 +1031,23 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>